<commit_message>
add entering next stage after removing all blocks function
</commit_message>
<xml_diff>
--- a/stages/stage_editor.xlsx
+++ b/stages/stage_editor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wojtek\Python\PyKanoid\stages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB9F9FE-B22F-46BC-AD6F-D0CF7E408265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D528ADF-F49C-4F65-A0C8-066E16F5BC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="5805" windowWidth="38700" windowHeight="15195" xr2:uid="{B6065C3E-5891-4ACC-B5E0-89174864E3F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B6065C3E-5891-4ACC-B5E0-89174864E3F0}"/>
   </bookViews>
   <sheets>
     <sheet name="standard_set" sheetId="1" r:id="rId1"/>
@@ -9575,7 +9575,7 @@
   <dimension ref="A1:T295"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="Y70" sqref="Y70"/>
+      <selection activeCell="AA85" sqref="AA85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>